<commit_message>
Made changes to NewLeadCreation code
</commit_message>
<xml_diff>
--- a/src/test/data/Lead_Data.xlsx
+++ b/src/test/data/Lead_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\IdeaProjects\SeleniumJava\SeleniumJava\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E3AFEC-5430-430F-B556-5AF55CCC35DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ADE1AC-B13D-4BBE-8A84-E72B3B5106C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>Joseph</t>
   </si>
@@ -152,6 +152,84 @@
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Advertisement</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Accenture</t>
+  </si>
+  <si>
+    <t>johndoe@accenture.com</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Hillary</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>Wipro</t>
+  </si>
+  <si>
+    <t>hdoe@wipro.com</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Customer Event</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Employee Referral</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>caleb@apple.ca</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>Caleb</t>
   </si>
 </sst>
 </file>
@@ -175,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +266,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -212,12 +296,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -225,6 +320,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -506,64 +604,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="19.6328125" customWidth="1"/>
-    <col min="5" max="5" width="28.54296875" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{73BFF79B-257D-4C7C-8493-13A234DD5034}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{73BFF79B-257D-4C7C-8493-13A234DD5034}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{F9982931-B28D-4C1C-9DEF-D1CE85CA2DF3}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{E481C6E4-05B8-478C-B381-1DAC6F34308D}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{5D4F2D02-1CD6-481D-B657-4CBCD979BD6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -573,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86903A2E-4CD9-499A-89EF-6277DAC73E2A}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="I1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>